<commit_message>
changed header names for import template
</commit_message>
<xml_diff>
--- a/Piccolo log tools/Piccolo Log Tools Import Template.xlsx
+++ b/Piccolo log tools/Piccolo Log Tools Import Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JAMES\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Repository\flight_analysis_tools\Piccolo log tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="401">
   <si>
     <t>Field:</t>
   </si>
@@ -142,15 +142,6 @@
     <t>qbar</t>
   </si>
   <si>
-    <t>pho</t>
-  </si>
-  <si>
-    <t>lon</t>
-  </si>
-  <si>
-    <t>lat</t>
-  </si>
-  <si>
     <t>ap_mode</t>
   </si>
   <si>
@@ -1186,18 +1177,6 @@
     <t>Altitude Mode</t>
   </si>
   <si>
-    <t>vel</t>
-  </si>
-  <si>
-    <t>veln</t>
-  </si>
-  <si>
-    <t>vele</t>
-  </si>
-  <si>
-    <t>veld</t>
-  </si>
-  <si>
     <t>Import Raw Surface Data</t>
   </si>
   <si>
@@ -1205,6 +1184,51 @@
   </si>
   <si>
     <t>raw data</t>
+  </si>
+  <si>
+    <t>velocity</t>
+  </si>
+  <si>
+    <t>velocity_n</t>
+  </si>
+  <si>
+    <t>velocity_e</t>
+  </si>
+  <si>
+    <t>velocity_d</t>
+  </si>
+  <si>
+    <t>roll_rate</t>
+  </si>
+  <si>
+    <t>pitch_rate</t>
+  </si>
+  <si>
+    <t>yaw_rate</t>
+  </si>
+  <si>
+    <t>a_x</t>
+  </si>
+  <si>
+    <t>a_y</t>
+  </si>
+  <si>
+    <t>a_z</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>dynamic_pressure</t>
+  </si>
+  <si>
+    <t>static_pressure</t>
+  </si>
+  <si>
+    <t>density</t>
   </si>
 </sst>
 </file>
@@ -1676,46 +1700,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.5703125" style="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" style="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" style="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="19" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" style="19" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" style="19" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="19" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="19" customWidth="1"/>
     <col min="8" max="8" width="10.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="16.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="12.5703125" style="19" customWidth="1"/>
-    <col min="21" max="21" width="10.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11" style="19" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.28515625" style="19" customWidth="1"/>
-    <col min="26" max="26" width="10" style="19" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.140625" style="19" customWidth="1"/>
-    <col min="29" max="29" width="14.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="15" style="19" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="19" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" style="19" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="19" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" style="19" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" style="19" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" style="19" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" style="19" customWidth="1"/>
+    <col min="16" max="17" width="13.5703125" style="19" customWidth="1"/>
+    <col min="18" max="18" width="11.28515625" style="19" customWidth="1"/>
+    <col min="19" max="19" width="12" style="19" customWidth="1"/>
+    <col min="20" max="20" width="8.140625" style="19" customWidth="1"/>
+    <col min="21" max="21" width="8.85546875" style="19" customWidth="1"/>
+    <col min="22" max="22" width="9.28515625" style="19" customWidth="1"/>
+    <col min="23" max="23" width="15.85546875" style="19" customWidth="1"/>
+    <col min="24" max="24" width="13.42578125" style="19" customWidth="1"/>
+    <col min="25" max="25" width="8.85546875" style="19" customWidth="1"/>
+    <col min="26" max="26" width="8" style="19" customWidth="1"/>
+    <col min="27" max="27" width="10" style="19" customWidth="1"/>
+    <col min="28" max="28" width="12" style="19" customWidth="1"/>
+    <col min="29" max="29" width="13.5703125" style="19" customWidth="1"/>
+    <col min="30" max="30" width="11.42578125" style="19" customWidth="1"/>
+    <col min="31" max="32" width="11.28515625" style="19" customWidth="1"/>
     <col min="33" max="33" width="19.28515625" style="19" bestFit="1" customWidth="1"/>
     <col min="34" max="43" width="9.5703125" style="19" bestFit="1" customWidth="1"/>
     <col min="44" max="49" width="10.5703125" style="19" bestFit="1" customWidth="1"/>
     <col min="50" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -1768,13 +1795,13 @@
         <v>13</v>
       </c>
       <c r="R1" s="21" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="S1" s="21" t="s">
+        <v>366</v>
+      </c>
+      <c r="T1" s="21" t="s">
         <v>369</v>
-      </c>
-      <c r="T1" s="21" t="s">
-        <v>372</v>
       </c>
       <c r="U1" s="21" t="s">
         <v>17</v>
@@ -1798,25 +1825,25 @@
         <v>19</v>
       </c>
       <c r="AB1" s="21" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="AC1" s="21" t="s">
+        <v>370</v>
+      </c>
+      <c r="AD1" s="21" t="s">
+        <v>372</v>
+      </c>
+      <c r="AE1" s="21" t="s">
         <v>373</v>
       </c>
-      <c r="AD1" s="21" t="s">
-        <v>375</v>
-      </c>
-      <c r="AE1" s="21" t="s">
-        <v>376</v>
-      </c>
       <c r="AF1" s="22" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="AG1" s="22" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="AH1" s="24" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="AI1" s="24"/>
       <c r="AJ1" s="24"/>
@@ -1860,13 +1887,13 @@
         <v>27</v>
       </c>
       <c r="I2" s="21" t="s">
-        <v>28</v>
+        <v>390</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>29</v>
+        <v>391</v>
       </c>
       <c r="K2" s="21" t="s">
-        <v>30</v>
+        <v>392</v>
       </c>
       <c r="L2" s="21" t="s">
         <v>31</v>
@@ -1878,64 +1905,64 @@
         <v>33</v>
       </c>
       <c r="O2" s="21" t="s">
-        <v>34</v>
+        <v>393</v>
       </c>
       <c r="P2" s="21" t="s">
-        <v>35</v>
+        <v>394</v>
       </c>
       <c r="Q2" s="21" t="s">
-        <v>36</v>
+        <v>395</v>
       </c>
       <c r="R2" s="21" t="s">
+        <v>365</v>
+      </c>
+      <c r="S2" s="21" t="s">
+        <v>367</v>
+      </c>
+      <c r="T2" s="21" t="s">
         <v>368</v>
       </c>
-      <c r="S2" s="21" t="s">
-        <v>370</v>
-      </c>
-      <c r="T2" s="21" t="s">
+      <c r="U2" s="21" t="s">
+        <v>396</v>
+      </c>
+      <c r="V2" s="21" t="s">
+        <v>397</v>
+      </c>
+      <c r="W2" s="21" t="s">
+        <v>398</v>
+      </c>
+      <c r="X2" s="21" t="s">
+        <v>399</v>
+      </c>
+      <c r="Y2" s="21" t="s">
+        <v>400</v>
+      </c>
+      <c r="Z2" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA2" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB2" s="21" t="s">
+        <v>381</v>
+      </c>
+      <c r="AC2" s="21" t="s">
         <v>371</v>
       </c>
-      <c r="U2" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="V2" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="W2" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="X2" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y2" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z2" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA2" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB2" s="21" t="s">
+      <c r="AD2" s="21" t="s">
+        <v>375</v>
+      </c>
+      <c r="AE2" s="21" t="s">
+        <v>376</v>
+      </c>
+      <c r="AF2" s="22" t="s">
+        <v>377</v>
+      </c>
+      <c r="AG2" s="22" t="s">
+        <v>379</v>
+      </c>
+      <c r="AH2" s="24" t="s">
         <v>384</v>
-      </c>
-      <c r="AC2" s="21" t="s">
-        <v>374</v>
-      </c>
-      <c r="AD2" s="21" t="s">
-        <v>378</v>
-      </c>
-      <c r="AE2" s="21" t="s">
-        <v>379</v>
-      </c>
-      <c r="AF2" s="22" t="s">
-        <v>380</v>
-      </c>
-      <c r="AG2" s="22" t="s">
-        <v>382</v>
-      </c>
-      <c r="AH2" s="24" t="s">
-        <v>391</v>
       </c>
       <c r="AI2" s="24"/>
       <c r="AJ2" s="24"/>
@@ -1955,104 +1982,104 @@
     </row>
     <row r="3" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="H3" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="J3" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="N3" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="O3" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="P3" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="Q3" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="G3" s="20" t="s">
+      <c r="R3" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="S3" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="T3" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="U3" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="V3" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="W3" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="X3" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="Y3" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="J3" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="K3" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="L3" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="M3" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="N3" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="O3" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="P3" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q3" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="R3" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="S3" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="T3" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="U3" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="V3" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="W3" s="21" t="s">
+      <c r="Z3" s="21" t="s">
         <v>49</v>
-      </c>
-      <c r="X3" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y3" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z3" s="21" t="s">
-        <v>52</v>
       </c>
       <c r="AA3" s="21"/>
       <c r="AB3" s="21" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="AC3" s="21" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="AD3" s="21" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="AE3" s="21" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="AF3" s="22" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="AG3" s="22" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="AH3" s="24" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="AI3" s="24"/>
       <c r="AJ3" s="24"/>
@@ -2072,151 +2099,151 @@
     </row>
     <row r="4" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>363</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="I4" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="J4" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="K4" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="G4" s="21" t="s">
-        <v>366</v>
-      </c>
-      <c r="H4" s="20" t="s">
+      <c r="L4" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="M4" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="N4" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="O4" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="P4" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="I4" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="J4" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="K4" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="L4" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="M4" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="N4" s="20" t="s">
+      <c r="Q4" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="O4" s="20" t="s">
+      <c r="R4" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="S4" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="T4" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="U4" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="V4" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="W4" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="P4" s="20" t="s">
+      <c r="X4" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="Q4" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="R4" s="20" t="s">
+      <c r="Y4" s="21" t="s">
+        <v>363</v>
+      </c>
+      <c r="Z4" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA4" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="S4" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="T4" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="U4" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="V4" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="W4" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="X4" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="Y4" s="21" t="s">
-        <v>366</v>
-      </c>
-      <c r="Z4" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA4" s="20" t="s">
-        <v>70</v>
-      </c>
       <c r="AB4" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="AC4" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD4" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="AE4" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="AF4" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="AC4" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="AD4" s="22" t="s">
-        <v>157</v>
-      </c>
-      <c r="AE4" s="22" t="s">
-        <v>158</v>
-      </c>
-      <c r="AF4" s="22" t="s">
-        <v>159</v>
-      </c>
       <c r="AG4" s="22" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="AH4" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="AI4" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="AJ4" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK4" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="AI4" s="23" t="s">
+      <c r="AL4" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="AJ4" s="23" t="s">
+      <c r="AM4" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="AK4" s="23" t="s">
+      <c r="AN4" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="AL4" s="23" t="s">
+      <c r="AO4" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="AM4" s="23" t="s">
+      <c r="AP4" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="AN4" s="23" t="s">
+      <c r="AQ4" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="AO4" s="23" t="s">
+      <c r="AR4" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="AP4" s="23" t="s">
+      <c r="AS4" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="AQ4" s="23" t="s">
+      <c r="AT4" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="AR4" s="23" t="s">
+      <c r="AU4" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="AS4" s="23" t="s">
+      <c r="AV4" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="AT4" s="23" t="s">
+      <c r="AW4" s="23" t="s">
         <v>121</v>
-      </c>
-      <c r="AU4" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="AV4" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="AW4" s="23" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:49" x14ac:dyDescent="0.2">
@@ -2413,670 +2440,670 @@
   <sheetData>
     <row r="1" spans="1:222" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="O1" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="T1" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="V1" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="W1" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="X1" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y1" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z1" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA1" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB1" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="AC1" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="AD1" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="AE1" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF1" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG1" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH1" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI1" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="AJ1" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="J1" s="16" t="s">
+      <c r="AK1" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL1" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM1" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN1" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="AO1" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="AP1" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="AQ1" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="AR1" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="AS1" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="AT1" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="AU1" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="AV1" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="AW1" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="AX1" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="AY1" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="AZ1" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="BA1" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="BB1" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="BC1" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="BD1" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="BE1" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="BF1" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="BG1" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="BH1" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="BI1" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="BJ1" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="BK1" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="BL1" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="BM1" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="BN1" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="BO1" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="BP1" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="BQ1" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="BR1" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="BS1" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="BT1" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="BU1" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="BV1" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="BW1" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="BX1" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="BY1" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="BZ1" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="CA1" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="CB1" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="CC1" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="CD1" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="K1" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="L1" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="M1" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="O1" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="P1" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q1" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="R1" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="S1" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="T1" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="U1" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="V1" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="W1" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="X1" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y1" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="Z1" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="AA1" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="AB1" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="AC1" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="AD1" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="AE1" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="AF1" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="AG1" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="AH1" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="AI1" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="AJ1" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="AK1" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="AL1" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM1" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="AN1" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="AO1" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="AP1" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="AQ1" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="AR1" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="AS1" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="AT1" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="AU1" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="AV1" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="AW1" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="AX1" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="AY1" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="AZ1" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="BA1" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="BB1" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="BC1" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="BD1" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="BE1" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="BF1" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="BG1" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="BH1" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="BI1" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="BJ1" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="BK1" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="BL1" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="BM1" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="BN1" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="BO1" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="BP1" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="BQ1" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="BR1" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="BS1" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="BT1" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="BU1" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="BV1" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="BW1" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="BX1" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="BY1" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="BZ1" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="CA1" s="10" t="s">
+      <c r="CE1" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="CB1" s="10" t="s">
+      <c r="CF1" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="CC1" s="10" t="s">
+      <c r="CG1" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="CD1" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="CE1" s="10" t="s">
+      <c r="CH1" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="CF1" s="10" t="s">
+      <c r="CI1" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="CG1" s="10" t="s">
+      <c r="CJ1" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="CH1" s="10" t="s">
+      <c r="CK1" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="CI1" s="10" t="s">
+      <c r="CL1" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="CJ1" s="10" t="s">
+      <c r="CM1" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="CK1" s="16" t="s">
+      <c r="CN1" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="CL1" s="10" t="s">
+      <c r="CO1" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="CM1" s="10" t="s">
+      <c r="CP1" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="CN1" s="10" t="s">
+      <c r="CQ1" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="CO1" s="10" t="s">
+      <c r="CR1" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="CP1" s="10" t="s">
+      <c r="CS1" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="CQ1" s="10" t="s">
+      <c r="CT1" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="CR1" s="10" t="s">
+      <c r="CU1" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="CS1" s="10" t="s">
+      <c r="CV1" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="CT1" s="10" t="s">
+      <c r="CW1" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="CU1" s="10" t="s">
+      <c r="CX1" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="CV1" s="10" t="s">
+      <c r="CY1" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="CW1" s="10" t="s">
+      <c r="CZ1" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="CX1" s="10" t="s">
+      <c r="DA1" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="CY1" s="16" t="s">
+      <c r="DB1" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="CZ1" s="16" t="s">
+      <c r="DC1" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="DA1" s="16" t="s">
+      <c r="DD1" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="DB1" s="16" t="s">
+      <c r="DE1" s="16" t="s">
         <v>159</v>
       </c>
-      <c r="DC1" s="16" t="s">
+      <c r="DF1" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="DD1" s="16" t="s">
+      <c r="DG1" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="DE1" s="16" t="s">
+      <c r="DH1" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="DF1" s="10" t="s">
+      <c r="DI1" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="DG1" s="10" t="s">
+      <c r="DJ1" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="DH1" s="10" t="s">
+      <c r="DK1" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="DI1" s="10" t="s">
+      <c r="DL1" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="DJ1" s="10" t="s">
+      <c r="DM1" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="DK1" s="10" t="s">
+      <c r="DN1" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="DL1" s="10" t="s">
+      <c r="DO1" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="DM1" s="10" t="s">
+      <c r="DP1" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="DN1" s="10" t="s">
+      <c r="DQ1" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="DO1" s="10" t="s">
+      <c r="DR1" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="DP1" s="10" t="s">
+      <c r="DS1" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="DQ1" s="10" t="s">
+      <c r="DT1" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="DR1" s="10" t="s">
+      <c r="DU1" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="DS1" s="10" t="s">
+      <c r="DV1" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="DT1" s="10" t="s">
+      <c r="DW1" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="DU1" s="10" t="s">
+      <c r="DX1" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="DV1" s="10" t="s">
+      <c r="DY1" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="DW1" s="10" t="s">
+      <c r="DZ1" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="DX1" s="10" t="s">
+      <c r="EA1" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="DY1" s="10" t="s">
+      <c r="EB1" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="DZ1" s="10" t="s">
+      <c r="EC1" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="EA1" s="10" t="s">
+      <c r="ED1" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="EB1" s="10" t="s">
+      <c r="EE1" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="EC1" s="10" t="s">
+      <c r="EF1" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="ED1" s="10" t="s">
+      <c r="EG1" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="EE1" s="10" t="s">
+      <c r="EH1" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="EF1" s="10" t="s">
+      <c r="EI1" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="EG1" s="10" t="s">
+      <c r="EJ1" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="EH1" s="10" t="s">
+      <c r="EK1" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="EI1" s="10" t="s">
+      <c r="EL1" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="EJ1" s="10" t="s">
+      <c r="EM1" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="EK1" s="10" t="s">
+      <c r="EN1" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="EL1" s="10" t="s">
+      <c r="EO1" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="EM1" s="10" t="s">
+      <c r="EP1" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="EN1" s="10" t="s">
+      <c r="EQ1" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="EO1" s="10" t="s">
+      <c r="ER1" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="EP1" s="10" t="s">
+      <c r="ES1" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="EQ1" s="10" t="s">
+      <c r="ET1" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="ER1" s="10" t="s">
+      <c r="EU1" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="ES1" s="10" t="s">
+      <c r="EV1" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="ET1" s="10" t="s">
+      <c r="EW1" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="EU1" s="10" t="s">
+      <c r="EX1" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="EV1" s="10" t="s">
+      <c r="EY1" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="EW1" s="10" t="s">
+      <c r="EZ1" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="EX1" s="10" t="s">
+      <c r="FA1" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="EY1" s="10" t="s">
+      <c r="FB1" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="EZ1" s="10" t="s">
+      <c r="FC1" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="FA1" s="10" t="s">
+      <c r="FD1" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="FB1" s="10" t="s">
+      <c r="FE1" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="FC1" s="10" t="s">
+      <c r="FF1" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="FD1" s="10" t="s">
+      <c r="FG1" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="FE1" s="10" t="s">
+      <c r="FH1" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="FF1" s="10" t="s">
+      <c r="FI1" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="FG1" s="10" t="s">
+      <c r="FJ1" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="FH1" s="10" t="s">
+      <c r="FK1" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="FI1" s="10" t="s">
+      <c r="FL1" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="FJ1" s="10" t="s">
+      <c r="FM1" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="FK1" s="10" t="s">
+      <c r="FN1" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="FL1" s="10" t="s">
+      <c r="FO1" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="FM1" s="10" t="s">
+      <c r="FP1" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="FN1" s="10" t="s">
+      <c r="FQ1" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="FO1" s="10" t="s">
+      <c r="FR1" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="FP1" s="10" t="s">
+      <c r="FS1" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="FQ1" s="10" t="s">
+      <c r="FT1" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="FR1" s="10" t="s">
+      <c r="FU1" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="FS1" s="10" t="s">
+      <c r="FV1" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="FT1" s="10" t="s">
+      <c r="FW1" s="10" t="s">
         <v>229</v>
       </c>
-      <c r="FU1" s="10" t="s">
+      <c r="FX1" s="10" t="s">
         <v>230</v>
       </c>
-      <c r="FV1" s="10" t="s">
+      <c r="FY1" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="FW1" s="10" t="s">
+      <c r="FZ1" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="FX1" s="10" t="s">
+      <c r="GA1" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="FY1" s="10" t="s">
+      <c r="GB1" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="FZ1" s="10" t="s">
+      <c r="GC1" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="GA1" s="10" t="s">
+      <c r="GD1" s="10" t="s">
         <v>236</v>
       </c>
-      <c r="GB1" s="10" t="s">
+      <c r="GE1" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="GC1" s="10" t="s">
+      <c r="GF1" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="GD1" s="10" t="s">
+      <c r="GG1" s="10" t="s">
         <v>239</v>
       </c>
-      <c r="GE1" s="10" t="s">
+      <c r="GH1" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="GF1" s="10" t="s">
+      <c r="GI1" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="GG1" s="10" t="s">
+      <c r="GJ1" s="10" t="s">
         <v>242</v>
       </c>
-      <c r="GH1" s="10" t="s">
+      <c r="GK1" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="GI1" s="10" t="s">
+      <c r="GL1" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="GJ1" s="10" t="s">
+      <c r="GM1" s="10" t="s">
         <v>245</v>
       </c>
-      <c r="GK1" s="10" t="s">
+      <c r="GN1" s="10" t="s">
         <v>246</v>
       </c>
-      <c r="GL1" s="10" t="s">
+      <c r="GO1" s="10" t="s">
         <v>247</v>
       </c>
-      <c r="GM1" s="10" t="s">
+      <c r="GP1" s="10" t="s">
         <v>248</v>
       </c>
-      <c r="GN1" s="10" t="s">
+      <c r="GQ1" s="10" t="s">
         <v>249</v>
       </c>
-      <c r="GO1" s="10" t="s">
+      <c r="GR1" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="GP1" s="10" t="s">
+      <c r="GS1" s="10" t="s">
         <v>251</v>
       </c>
-      <c r="GQ1" s="10" t="s">
+      <c r="GT1" s="10" t="s">
         <v>252</v>
       </c>
-      <c r="GR1" s="10" t="s">
+      <c r="GU1" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="GS1" s="10" t="s">
+      <c r="GV1" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="GT1" s="10" t="s">
+      <c r="GW1" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="GU1" s="10" t="s">
+      <c r="GX1" s="10" t="s">
         <v>256</v>
       </c>
-      <c r="GV1" s="10" t="s">
+      <c r="GY1" s="10" t="s">
         <v>257</v>
       </c>
-      <c r="GW1" s="10" t="s">
+      <c r="GZ1" s="10" t="s">
         <v>258</v>
       </c>
-      <c r="GX1" s="10" t="s">
+      <c r="HA1" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="GY1" s="10" t="s">
+      <c r="HB1" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="GZ1" s="10" t="s">
+      <c r="HC1" s="10" t="s">
         <v>261</v>
       </c>
-      <c r="HA1" s="10" t="s">
+      <c r="HD1" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="HB1" s="10" t="s">
+      <c r="HE1" s="10" t="s">
         <v>263</v>
       </c>
-      <c r="HC1" s="10" t="s">
+      <c r="HF1" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="HD1" s="10" t="s">
+      <c r="HG1" s="10" t="s">
         <v>265</v>
       </c>
-      <c r="HE1" s="10" t="s">
+      <c r="HH1" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="HF1" s="10" t="s">
+      <c r="HI1" s="10" t="s">
         <v>267</v>
       </c>
-      <c r="HG1" s="10" t="s">
+      <c r="HJ1" s="10" t="s">
         <v>268</v>
       </c>
-      <c r="HH1" s="10" t="s">
+      <c r="HK1" s="10" t="s">
         <v>269</v>
       </c>
-      <c r="HI1" s="10" t="s">
+      <c r="HL1" s="10" t="s">
         <v>270</v>
       </c>
-      <c r="HJ1" s="10" t="s">
+      <c r="HM1" s="10" t="s">
         <v>271</v>
       </c>
-      <c r="HK1" s="10" t="s">
+      <c r="HN1" s="10" t="s">
         <v>272</v>
-      </c>
-      <c r="HL1" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="HM1" s="10" t="s">
-        <v>274</v>
-      </c>
-      <c r="HN1" s="10" t="s">
-        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -3101,13 +3128,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3118,7 +3145,7 @@
         <v>25</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3126,10 +3153,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3140,7 +3167,7 @@
         <v>26</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3151,7 +3178,7 @@
         <v>27</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3162,7 +3189,7 @@
         <v>28</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3173,7 +3200,7 @@
         <v>29</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3184,7 +3211,7 @@
         <v>30</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3192,10 +3219,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3203,10 +3230,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3214,10 +3241,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3228,7 +3255,7 @@
         <v>34</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3239,7 +3266,7 @@
         <v>35</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3250,7 +3277,7 @@
         <v>36</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3258,10 +3285,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3269,10 +3296,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3280,10 +3307,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3291,10 +3318,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3302,10 +3329,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3313,10 +3340,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3324,10 +3351,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3335,10 +3362,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3346,10 +3373,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3357,10 +3384,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3368,10 +3395,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3379,10 +3406,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3390,10 +3417,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3404,7 +3431,7 @@
         <v>37</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3412,10 +3439,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3423,10 +3450,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3434,10 +3461,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3445,10 +3472,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3456,10 +3483,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3467,10 +3494,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3478,10 +3505,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3489,10 +3516,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3500,10 +3527,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3511,10 +3538,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3522,10 +3549,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3533,10 +3560,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3544,10 +3571,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3555,10 +3582,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3566,10 +3593,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3577,10 +3604,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3588,10 +3615,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3599,10 +3626,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3610,10 +3637,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3621,10 +3648,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3632,10 +3659,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3643,10 +3670,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3654,10 +3681,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3665,10 +3692,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3676,10 +3703,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3687,10 +3714,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3698,10 +3725,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3709,10 +3736,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3720,10 +3747,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3731,10 +3758,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3742,10 +3769,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3753,10 +3780,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3764,10 +3791,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3775,10 +3802,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3786,10 +3813,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3797,10 +3824,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3808,10 +3835,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3819,10 +3846,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3830,10 +3857,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3841,10 +3868,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3852,10 +3879,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3863,10 +3890,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3874,10 +3901,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3885,10 +3912,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3896,10 +3923,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3907,10 +3934,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3918,10 +3945,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3929,10 +3956,10 @@
         <v>75</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3940,10 +3967,10 @@
         <v>76</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3951,10 +3978,10 @@
         <v>77</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3962,10 +3989,10 @@
         <v>78</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3973,10 +4000,10 @@
         <v>79</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3984,10 +4011,10 @@
         <v>80</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3995,10 +4022,10 @@
         <v>81</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
changes to header names
</commit_message>
<xml_diff>
--- a/Piccolo log tools/Piccolo Log Tools Import Template.xlsx
+++ b/Piccolo log tools/Piccolo Log Tools Import Template.xlsx
@@ -26,17 +26,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="401">
-  <si>
-    <t>Field:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="400">
   <si>
     <t>Time</t>
   </si>
   <si>
-    <t>Velocity</t>
-  </si>
-  <si>
     <t>Beta</t>
   </si>
   <si>
@@ -1168,15 +1162,6 @@
     <t>vel_track</t>
   </si>
   <si>
-    <t>mag of velocity tackers</t>
-  </si>
-  <si>
-    <t>alt_mode</t>
-  </si>
-  <si>
-    <t>Altitude Mode</t>
-  </si>
-  <si>
     <t>Import Raw Surface Data</t>
   </si>
   <si>
@@ -1186,18 +1171,6 @@
     <t>raw data</t>
   </si>
   <si>
-    <t>velocity</t>
-  </si>
-  <si>
-    <t>velocity_n</t>
-  </si>
-  <si>
-    <t>velocity_e</t>
-  </si>
-  <si>
-    <t>velocity_d</t>
-  </si>
-  <si>
     <t>roll_rate</t>
   </si>
   <si>
@@ -1228,7 +1201,31 @@
     <t>static_pressure</t>
   </si>
   <si>
-    <t>density</t>
+    <t>velocity_north</t>
+  </si>
+  <si>
+    <t>velocity_east</t>
+  </si>
+  <si>
+    <t>velocity_down</t>
+  </si>
+  <si>
+    <t>Descirption</t>
+  </si>
+  <si>
+    <t>tas</t>
+  </si>
+  <si>
+    <t>TAS</t>
+  </si>
+  <si>
+    <t>density_air</t>
+  </si>
+  <si>
+    <t>alt_ctrl</t>
+  </si>
+  <si>
+    <t>Altitude Control</t>
   </si>
 </sst>
 </file>
@@ -1368,7 +1365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1418,6 +1415,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1700,8 +1698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AH4" sqref="AH4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1729,14 +1727,13 @@
     <col min="22" max="22" width="9.28515625" style="19" customWidth="1"/>
     <col min="23" max="23" width="15.85546875" style="19" customWidth="1"/>
     <col min="24" max="24" width="13.42578125" style="19" customWidth="1"/>
-    <col min="25" max="25" width="8.85546875" style="19" customWidth="1"/>
+    <col min="25" max="25" width="9.7109375" style="19" customWidth="1"/>
     <col min="26" max="26" width="8" style="19" customWidth="1"/>
     <col min="27" max="27" width="10" style="19" customWidth="1"/>
-    <col min="28" max="28" width="12" style="19" customWidth="1"/>
-    <col min="29" max="29" width="13.5703125" style="19" customWidth="1"/>
+    <col min="28" max="29" width="13.5703125" style="19" customWidth="1"/>
     <col min="30" max="30" width="11.42578125" style="19" customWidth="1"/>
     <col min="31" max="32" width="11.28515625" style="19" customWidth="1"/>
-    <col min="33" max="33" width="19.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.7109375" style="19" bestFit="1" customWidth="1"/>
     <col min="34" max="43" width="9.5703125" style="19" bestFit="1" customWidth="1"/>
     <col min="44" max="49" width="10.5703125" style="19" bestFit="1" customWidth="1"/>
     <col min="50" max="16384" width="9.140625" style="19"/>
@@ -1744,106 +1741,106 @@
   <sheetData>
     <row r="1" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
+        <v>394</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="C1" s="20" t="s">
+        <v>396</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="H1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="20" t="s">
+      <c r="I1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="K1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="L1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="M1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="N1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="O1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="P1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="Q1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="21" t="s">
+      <c r="R1" s="21" t="s">
+        <v>362</v>
+      </c>
+      <c r="S1" s="21" t="s">
+        <v>364</v>
+      </c>
+      <c r="T1" s="21" t="s">
+        <v>367</v>
+      </c>
+      <c r="U1" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="V1" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="W1" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="21" t="s">
+      <c r="X1" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="21" t="s">
-        <v>364</v>
-      </c>
-      <c r="S1" s="21" t="s">
-        <v>366</v>
-      </c>
-      <c r="T1" s="21" t="s">
-        <v>369</v>
-      </c>
-      <c r="U1" s="21" t="s">
+      <c r="Y1" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z1" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA1" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="W1" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="X1" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y1" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z1" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA1" s="21" t="s">
-        <v>19</v>
-      </c>
       <c r="AB1" s="21" t="s">
-        <v>382</v>
+        <v>399</v>
       </c>
       <c r="AC1" s="21" t="s">
+        <v>368</v>
+      </c>
+      <c r="AD1" s="21" t="s">
         <v>370</v>
       </c>
-      <c r="AD1" s="21" t="s">
+      <c r="AE1" s="21" t="s">
+        <v>371</v>
+      </c>
+      <c r="AF1" s="22" t="s">
         <v>372</v>
       </c>
-      <c r="AE1" s="21" t="s">
-        <v>373</v>
-      </c>
-      <c r="AF1" s="22" t="s">
-        <v>374</v>
-      </c>
       <c r="AG1" s="22" t="s">
+        <v>376</v>
+      </c>
+      <c r="AH1" s="24" t="s">
         <v>378</v>
-      </c>
-      <c r="AH1" s="24" t="s">
-        <v>383</v>
       </c>
       <c r="AI1" s="24"/>
       <c r="AJ1" s="24"/>
@@ -1861,108 +1858,108 @@
       <c r="AV1" s="24"/>
       <c r="AW1" s="24"/>
     </row>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:49" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>395</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>391</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>392</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>393</v>
+      </c>
+      <c r="G2" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="H2" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="I2" s="21" t="s">
+        <v>381</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>382</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>383</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="21" t="s">
+        <v>384</v>
+      </c>
+      <c r="P2" s="21" t="s">
+        <v>385</v>
+      </c>
+      <c r="Q2" s="21" t="s">
         <v>386</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="R2" s="21" t="s">
+        <v>363</v>
+      </c>
+      <c r="S2" s="21" t="s">
+        <v>365</v>
+      </c>
+      <c r="T2" s="21" t="s">
+        <v>366</v>
+      </c>
+      <c r="U2" s="21" t="s">
         <v>387</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="V2" s="21" t="s">
         <v>388</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="W2" s="21" t="s">
         <v>389</v>
       </c>
-      <c r="G2" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" s="21" t="s">
+      <c r="X2" s="21" t="s">
         <v>390</v>
       </c>
-      <c r="J2" s="21" t="s">
-        <v>391</v>
-      </c>
-      <c r="K2" s="21" t="s">
-        <v>392</v>
-      </c>
-      <c r="L2" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="M2" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="N2" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="O2" s="21" t="s">
-        <v>393</v>
-      </c>
-      <c r="P2" s="21" t="s">
-        <v>394</v>
-      </c>
-      <c r="Q2" s="21" t="s">
-        <v>395</v>
-      </c>
-      <c r="R2" s="21" t="s">
-        <v>365</v>
-      </c>
-      <c r="S2" s="21" t="s">
-        <v>367</v>
-      </c>
-      <c r="T2" s="21" t="s">
-        <v>368</v>
-      </c>
-      <c r="U2" s="21" t="s">
-        <v>396</v>
-      </c>
-      <c r="V2" s="21" t="s">
+      <c r="Y2" s="21" t="s">
         <v>397</v>
       </c>
-      <c r="W2" s="21" t="s">
+      <c r="Z2" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA2" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB2" s="21" t="s">
         <v>398</v>
       </c>
-      <c r="X2" s="21" t="s">
-        <v>399</v>
-      </c>
-      <c r="Y2" s="21" t="s">
-        <v>400</v>
-      </c>
-      <c r="Z2" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA2" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB2" s="21" t="s">
-        <v>381</v>
-      </c>
       <c r="AC2" s="21" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="AD2" s="21" t="s">
+        <v>373</v>
+      </c>
+      <c r="AE2" s="21" t="s">
+        <v>374</v>
+      </c>
+      <c r="AF2" s="22" t="s">
         <v>375</v>
       </c>
-      <c r="AE2" s="21" t="s">
-        <v>376</v>
-      </c>
-      <c r="AF2" s="22" t="s">
+      <c r="AG2" s="22" t="s">
         <v>377</v>
       </c>
-      <c r="AG2" s="22" t="s">
+      <c r="AH2" s="24" t="s">
         <v>379</v>
-      </c>
-      <c r="AH2" s="24" t="s">
-        <v>384</v>
       </c>
       <c r="AI2" s="24"/>
       <c r="AJ2" s="24"/>
@@ -1982,104 +1979,104 @@
     </row>
     <row r="3" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="D3" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="H3" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="J3" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="K3" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" s="20" t="s">
+      <c r="L3" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="N3" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="P3" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="Q3" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="R3" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="S3" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="T3" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="U3" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="V3" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="W3" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="J3" s="21" t="s">
+      <c r="X3" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="K3" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="L3" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="M3" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="N3" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="O3" s="21" t="s">
+      <c r="Y3" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="P3" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q3" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="R3" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="S3" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="T3" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="U3" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="V3" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="W3" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="X3" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y3" s="21" t="s">
+      <c r="Z3" s="21" t="s">
         <v>47</v>
-      </c>
-      <c r="Z3" s="21" t="s">
-        <v>49</v>
       </c>
       <c r="AA3" s="21"/>
       <c r="AB3" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="AC3" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="AD3" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="AE3" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="AF3" s="22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="AG3" s="22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="AH3" s="24" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="AI3" s="24"/>
       <c r="AJ3" s="24"/>
@@ -2099,151 +2096,151 @@
     </row>
     <row r="4" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="D4" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>361</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="I4" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="J4" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="G4" s="21" t="s">
-        <v>363</v>
-      </c>
-      <c r="H4" s="20" t="s">
+      <c r="K4" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="M4" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N4" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="O4" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="I4" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="J4" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="K4" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="L4" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="M4" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="N4" s="20" t="s">
+      <c r="P4" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="O4" s="20" t="s">
+      <c r="Q4" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="P4" s="20" t="s">
+      <c r="R4" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="S4" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="T4" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="U4" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="V4" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="W4" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="Q4" s="20" t="s">
+      <c r="X4" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="R4" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="S4" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="T4" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="U4" s="20" t="s">
+      <c r="Y4" s="21" t="s">
+        <v>361</v>
+      </c>
+      <c r="Z4" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA4" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="V4" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="W4" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="X4" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y4" s="21" t="s">
-        <v>363</v>
-      </c>
-      <c r="Z4" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA4" s="20" t="s">
-        <v>67</v>
-      </c>
       <c r="AB4" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC4" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="AD4" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="AE4" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="AC4" s="22" t="s">
-        <v>140</v>
-      </c>
-      <c r="AD4" s="22" t="s">
+      <c r="AF4" s="22" t="s">
         <v>154</v>
       </c>
-      <c r="AE4" s="22" t="s">
-        <v>155</v>
-      </c>
-      <c r="AF4" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="AG4" s="22" t="s">
-        <v>380</v>
+      <c r="AG4" s="25" t="s">
+        <v>136</v>
       </c>
       <c r="AH4" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="AI4" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="AJ4" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="AI4" s="23" t="s">
+      <c r="AK4" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="AJ4" s="23" t="s">
+      <c r="AL4" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="AK4" s="23" t="s">
+      <c r="AM4" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="AL4" s="23" t="s">
+      <c r="AN4" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="AM4" s="23" t="s">
+      <c r="AO4" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="AN4" s="23" t="s">
+      <c r="AP4" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="AO4" s="23" t="s">
+      <c r="AQ4" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="AP4" s="23" t="s">
+      <c r="AR4" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="AQ4" s="23" t="s">
+      <c r="AS4" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="AR4" s="23" t="s">
+      <c r="AT4" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="AS4" s="23" t="s">
+      <c r="AU4" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="AT4" s="23" t="s">
+      <c r="AV4" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="AU4" s="23" t="s">
+      <c r="AW4" s="23" t="s">
         <v>119</v>
-      </c>
-      <c r="AV4" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="AW4" s="23" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:49" x14ac:dyDescent="0.2">
@@ -2440,670 +2437,670 @@
   <sheetData>
     <row r="1" spans="1:222" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="O1" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="T1" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="V1" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="W1" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="X1" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y1" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA1" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="AB1" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC1" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD1" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="AE1" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF1" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG1" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH1" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI1" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="H1" s="16" t="s">
+      <c r="AJ1" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK1" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="AL1" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="AM1" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN1" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="AO1" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP1" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="AQ1" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="AR1" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="AS1" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="AT1" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="AU1" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="AV1" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="AW1" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="AX1" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="AY1" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="AZ1" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="BA1" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="BB1" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="BC1" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="BD1" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="BE1" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="BF1" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="BG1" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="BH1" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="BI1" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="BJ1" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="BK1" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="BL1" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="BM1" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="BN1" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="BO1" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="BP1" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="BQ1" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="BR1" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="BS1" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="BT1" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="BU1" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="BV1" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="BW1" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="BX1" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="BY1" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="BZ1" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="CA1" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="CB1" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="CC1" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="CD1" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="I1" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="J1" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="K1" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="L1" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="M1" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="O1" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="P1" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q1" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="R1" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="S1" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="T1" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="U1" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="V1" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="W1" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="X1" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="Y1" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="Z1" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="AA1" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="AB1" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="AC1" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="AD1" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="AE1" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="AF1" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="AG1" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="AH1" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="AI1" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="AJ1" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="AK1" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="AL1" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="AM1" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="AN1" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="AO1" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="AP1" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="AQ1" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="AR1" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="AS1" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="AT1" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="AU1" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="AV1" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="AW1" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="AX1" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="AY1" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="AZ1" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="BA1" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="BB1" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="BC1" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="BD1" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="BE1" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="BF1" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="BG1" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="BH1" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="BI1" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="BJ1" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="BK1" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="BL1" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="BM1" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="BN1" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="BO1" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="BP1" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="BQ1" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="BR1" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="BS1" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="BT1" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="BU1" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="BV1" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="BW1" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="BX1" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="BY1" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="BZ1" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="CA1" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="CB1" s="10" t="s">
+      <c r="CE1" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="CC1" s="10" t="s">
+      <c r="CF1" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="CD1" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="CE1" s="10" t="s">
+      <c r="CG1" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="CF1" s="10" t="s">
+      <c r="CH1" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="CG1" s="10" t="s">
+      <c r="CI1" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="CH1" s="10" t="s">
+      <c r="CJ1" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="CI1" s="10" t="s">
+      <c r="CK1" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="CJ1" s="10" t="s">
+      <c r="CL1" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="CK1" s="16" t="s">
+      <c r="CM1" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="CL1" s="10" t="s">
+      <c r="CN1" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="CM1" s="10" t="s">
+      <c r="CO1" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="CN1" s="10" t="s">
+      <c r="CP1" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="CO1" s="10" t="s">
+      <c r="CQ1" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="CP1" s="10" t="s">
+      <c r="CR1" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="CQ1" s="10" t="s">
+      <c r="CS1" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="CR1" s="10" t="s">
+      <c r="CT1" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="CS1" s="10" t="s">
+      <c r="CU1" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="CT1" s="10" t="s">
+      <c r="CV1" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="CU1" s="10" t="s">
+      <c r="CW1" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="CV1" s="10" t="s">
+      <c r="CX1" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="CW1" s="10" t="s">
+      <c r="CY1" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="CX1" s="10" t="s">
+      <c r="CZ1" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="CY1" s="16" t="s">
+      <c r="DA1" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="CZ1" s="16" t="s">
+      <c r="DB1" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="DA1" s="16" t="s">
+      <c r="DC1" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="DB1" s="16" t="s">
+      <c r="DD1" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="DC1" s="16" t="s">
+      <c r="DE1" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="DD1" s="16" t="s">
+      <c r="DF1" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="DE1" s="16" t="s">
+      <c r="DG1" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="DF1" s="10" t="s">
+      <c r="DH1" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="DG1" s="10" t="s">
+      <c r="DI1" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="DH1" s="10" t="s">
+      <c r="DJ1" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="DI1" s="10" t="s">
+      <c r="DK1" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="DJ1" s="10" t="s">
+      <c r="DL1" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="DK1" s="10" t="s">
+      <c r="DM1" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="DL1" s="10" t="s">
+      <c r="DN1" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="DM1" s="10" t="s">
+      <c r="DO1" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="DN1" s="10" t="s">
+      <c r="DP1" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="DO1" s="10" t="s">
+      <c r="DQ1" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="DP1" s="10" t="s">
+      <c r="DR1" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="DQ1" s="10" t="s">
+      <c r="DS1" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="DR1" s="10" t="s">
+      <c r="DT1" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="DS1" s="10" t="s">
+      <c r="DU1" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="DT1" s="10" t="s">
+      <c r="DV1" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="DU1" s="10" t="s">
+      <c r="DW1" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="DV1" s="10" t="s">
+      <c r="DX1" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="DW1" s="10" t="s">
+      <c r="DY1" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="DX1" s="10" t="s">
+      <c r="DZ1" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="DY1" s="10" t="s">
+      <c r="EA1" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="DZ1" s="10" t="s">
+      <c r="EB1" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="EA1" s="10" t="s">
+      <c r="EC1" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="EB1" s="10" t="s">
+      <c r="ED1" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="EC1" s="10" t="s">
+      <c r="EE1" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="ED1" s="10" t="s">
+      <c r="EF1" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="EE1" s="10" t="s">
+      <c r="EG1" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="EF1" s="10" t="s">
+      <c r="EH1" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="EG1" s="10" t="s">
+      <c r="EI1" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="EH1" s="10" t="s">
+      <c r="EJ1" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="EI1" s="10" t="s">
+      <c r="EK1" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="EJ1" s="10" t="s">
+      <c r="EL1" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="EK1" s="10" t="s">
+      <c r="EM1" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="EL1" s="10" t="s">
+      <c r="EN1" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="EM1" s="10" t="s">
+      <c r="EO1" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="EN1" s="10" t="s">
+      <c r="EP1" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="EO1" s="10" t="s">
+      <c r="EQ1" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="EP1" s="10" t="s">
+      <c r="ER1" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="EQ1" s="10" t="s">
+      <c r="ES1" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="ER1" s="10" t="s">
+      <c r="ET1" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="ES1" s="10" t="s">
+      <c r="EU1" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="ET1" s="10" t="s">
+      <c r="EV1" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="EU1" s="10" t="s">
+      <c r="EW1" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="EV1" s="10" t="s">
+      <c r="EX1" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="EW1" s="10" t="s">
+      <c r="EY1" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="EX1" s="10" t="s">
+      <c r="EZ1" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="EY1" s="10" t="s">
+      <c r="FA1" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="EZ1" s="10" t="s">
+      <c r="FB1" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="FA1" s="10" t="s">
+      <c r="FC1" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="FB1" s="10" t="s">
+      <c r="FD1" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="FC1" s="10" t="s">
+      <c r="FE1" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="FD1" s="10" t="s">
+      <c r="FF1" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="FE1" s="10" t="s">
+      <c r="FG1" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="FF1" s="10" t="s">
+      <c r="FH1" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="FG1" s="10" t="s">
+      <c r="FI1" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="FH1" s="10" t="s">
+      <c r="FJ1" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="FI1" s="10" t="s">
+      <c r="FK1" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="FJ1" s="10" t="s">
+      <c r="FL1" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="FK1" s="10" t="s">
+      <c r="FM1" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="FL1" s="10" t="s">
+      <c r="FN1" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="FM1" s="10" t="s">
+      <c r="FO1" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="FN1" s="10" t="s">
+      <c r="FP1" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="FO1" s="10" t="s">
+      <c r="FQ1" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="FP1" s="10" t="s">
+      <c r="FR1" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="FQ1" s="10" t="s">
+      <c r="FS1" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="FR1" s="10" t="s">
+      <c r="FT1" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="FS1" s="10" t="s">
+      <c r="FU1" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="FT1" s="10" t="s">
+      <c r="FV1" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="FU1" s="10" t="s">
+      <c r="FW1" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="FV1" s="10" t="s">
+      <c r="FX1" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="FW1" s="10" t="s">
+      <c r="FY1" s="10" t="s">
         <v>229</v>
       </c>
-      <c r="FX1" s="10" t="s">
+      <c r="FZ1" s="10" t="s">
         <v>230</v>
       </c>
-      <c r="FY1" s="10" t="s">
+      <c r="GA1" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="FZ1" s="10" t="s">
+      <c r="GB1" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="GA1" s="10" t="s">
+      <c r="GC1" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="GB1" s="10" t="s">
+      <c r="GD1" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="GC1" s="10" t="s">
+      <c r="GE1" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="GD1" s="10" t="s">
+      <c r="GF1" s="10" t="s">
         <v>236</v>
       </c>
-      <c r="GE1" s="10" t="s">
+      <c r="GG1" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="GF1" s="10" t="s">
+      <c r="GH1" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="GG1" s="10" t="s">
+      <c r="GI1" s="10" t="s">
         <v>239</v>
       </c>
-      <c r="GH1" s="10" t="s">
+      <c r="GJ1" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="GI1" s="10" t="s">
+      <c r="GK1" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="GJ1" s="10" t="s">
+      <c r="GL1" s="10" t="s">
         <v>242</v>
       </c>
-      <c r="GK1" s="10" t="s">
+      <c r="GM1" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="GL1" s="10" t="s">
+      <c r="GN1" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="GM1" s="10" t="s">
+      <c r="GO1" s="10" t="s">
         <v>245</v>
       </c>
-      <c r="GN1" s="10" t="s">
+      <c r="GP1" s="10" t="s">
         <v>246</v>
       </c>
-      <c r="GO1" s="10" t="s">
+      <c r="GQ1" s="10" t="s">
         <v>247</v>
       </c>
-      <c r="GP1" s="10" t="s">
+      <c r="GR1" s="10" t="s">
         <v>248</v>
       </c>
-      <c r="GQ1" s="10" t="s">
+      <c r="GS1" s="10" t="s">
         <v>249</v>
       </c>
-      <c r="GR1" s="10" t="s">
+      <c r="GT1" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="GS1" s="10" t="s">
+      <c r="GU1" s="10" t="s">
         <v>251</v>
       </c>
-      <c r="GT1" s="10" t="s">
+      <c r="GV1" s="10" t="s">
         <v>252</v>
       </c>
-      <c r="GU1" s="10" t="s">
+      <c r="GW1" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="GV1" s="10" t="s">
+      <c r="GX1" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="GW1" s="10" t="s">
+      <c r="GY1" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="GX1" s="10" t="s">
+      <c r="GZ1" s="10" t="s">
         <v>256</v>
       </c>
-      <c r="GY1" s="10" t="s">
+      <c r="HA1" s="10" t="s">
         <v>257</v>
       </c>
-      <c r="GZ1" s="10" t="s">
+      <c r="HB1" s="10" t="s">
         <v>258</v>
       </c>
-      <c r="HA1" s="10" t="s">
+      <c r="HC1" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="HB1" s="10" t="s">
+      <c r="HD1" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="HC1" s="10" t="s">
+      <c r="HE1" s="10" t="s">
         <v>261</v>
       </c>
-      <c r="HD1" s="10" t="s">
+      <c r="HF1" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="HE1" s="10" t="s">
+      <c r="HG1" s="10" t="s">
         <v>263</v>
       </c>
-      <c r="HF1" s="10" t="s">
+      <c r="HH1" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="HG1" s="10" t="s">
+      <c r="HI1" s="10" t="s">
         <v>265</v>
       </c>
-      <c r="HH1" s="10" t="s">
+      <c r="HJ1" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="HI1" s="10" t="s">
+      <c r="HK1" s="10" t="s">
         <v>267</v>
       </c>
-      <c r="HJ1" s="10" t="s">
+      <c r="HL1" s="10" t="s">
         <v>268</v>
       </c>
-      <c r="HK1" s="10" t="s">
+      <c r="HM1" s="10" t="s">
         <v>269</v>
       </c>
-      <c r="HL1" s="10" t="s">
+      <c r="HN1" s="10" t="s">
         <v>270</v>
-      </c>
-      <c r="HM1" s="10" t="s">
-        <v>271</v>
-      </c>
-      <c r="HN1" s="10" t="s">
-        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -3128,13 +3125,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>273</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3142,10 +3139,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3153,10 +3150,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3164,10 +3161,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3175,10 +3172,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3186,10 +3183,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3197,10 +3194,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3208,10 +3205,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3219,10 +3216,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3230,10 +3227,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3241,10 +3238,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3252,10 +3249,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3263,10 +3260,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3274,10 +3271,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3285,10 +3282,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3296,10 +3293,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3307,10 +3304,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3318,10 +3315,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3329,10 +3326,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3340,10 +3337,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3351,10 +3348,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3362,10 +3359,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3373,10 +3370,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3384,10 +3381,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3395,10 +3392,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3406,10 +3403,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3417,10 +3414,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3428,10 +3425,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3439,10 +3436,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3450,10 +3447,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3461,10 +3458,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3472,10 +3469,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3483,10 +3480,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3494,10 +3491,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3505,10 +3502,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3516,10 +3513,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3527,10 +3524,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3538,10 +3535,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3549,10 +3546,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3560,10 +3557,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3571,10 +3568,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3582,10 +3579,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3593,10 +3590,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3604,10 +3601,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3615,10 +3612,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3626,10 +3623,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3637,10 +3634,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3648,10 +3645,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3659,10 +3656,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3670,10 +3667,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3681,10 +3678,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3692,10 +3689,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3703,10 +3700,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3714,10 +3711,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3725,10 +3722,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3736,10 +3733,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3747,10 +3744,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3758,10 +3755,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3769,10 +3766,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3780,10 +3777,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3791,10 +3788,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3802,10 +3799,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3813,10 +3810,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3824,10 +3821,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3835,10 +3832,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3846,10 +3843,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3857,10 +3854,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3868,10 +3865,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3879,10 +3876,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3890,10 +3887,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3901,10 +3898,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3912,10 +3909,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3923,10 +3920,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3934,10 +3931,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3945,10 +3942,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3956,10 +3953,10 @@
         <v>75</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3967,10 +3964,10 @@
         <v>76</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3978,10 +3975,10 @@
         <v>77</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3989,10 +3986,10 @@
         <v>78</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4000,10 +3997,10 @@
         <v>79</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4011,10 +4008,10 @@
         <v>80</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4022,10 +4019,10 @@
         <v>81</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>